<commit_message>
begin to write method
</commit_message>
<xml_diff>
--- a/paperWriting/Method/MethodTable.xlsx
+++ b/paperWriting/Method/MethodTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="2180" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="7980" yWindow="20" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,181 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+  <si>
+    <t>compond</t>
+  </si>
+  <si>
+    <t>GOC</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>data source/ data set</t>
+  </si>
+  <si>
+    <t>feature</t>
+  </si>
+  <si>
+    <t>Shared
+Annotation</t>
+  </si>
+  <si>
+    <t>Homologous
+Interactions</t>
+  </si>
+  <si>
+    <t>statistics</t>
+  </si>
+  <si>
+    <t>Max Shared
+Annotaion
+Score</t>
+  </si>
+  <si>
+    <t>Inparanoid Homologous Score Set</t>
+  </si>
+  <si>
+    <t>Blast Homologous Score Set</t>
+  </si>
+  <si>
+    <t>Max Homologous
+Score</t>
+  </si>
+  <si>
+    <t>3did</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>DPEA</t>
+  </si>
+  <si>
+    <t>iPfam</t>
+  </si>
+  <si>
+    <t>RCDP</t>
+  </si>
+  <si>
+    <t>Pvalue</t>
+  </si>
+  <si>
+    <t>Fusion</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>GPE</t>
+  </si>
+  <si>
+    <t>DIPD</t>
+  </si>
+  <si>
+    <t>RDFF</t>
+  </si>
+  <si>
+    <t>KGIDDI</t>
+  </si>
+  <si>
+    <t>INSITE</t>
+  </si>
+  <si>
+    <t>DomainGA</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>Max Shared
+Domain
+Score</t>
+  </si>
+  <si>
+    <t>Domain
+Interaction</t>
+  </si>
+  <si>
+    <t>Colocalization</t>
+  </si>
+  <si>
+    <t>SUBA3</t>
+  </si>
+  <si>
+    <t>Tanimato Correlation</t>
+  </si>
+  <si>
+    <t>Co-expression</t>
+  </si>
+  <si>
+    <t>Weigel
+World</t>
+  </si>
+  <si>
+    <t>pathogen</t>
+  </si>
+  <si>
+    <t>development</t>
+  </si>
+  <si>
+    <t>abiotic stress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light </t>
+  </si>
+  <si>
+    <t>ecotype</t>
+  </si>
+  <si>
+    <t>TAIR</t>
+  </si>
+  <si>
+    <t>Pearsons Correlation</t>
+  </si>
+  <si>
+    <t>Phylogenetic
+Profile</t>
+  </si>
+  <si>
+    <t>ROUNDUP</t>
+  </si>
+  <si>
+    <t>Mutual Information</t>
+  </si>
+  <si>
+    <t>Pearson's Correlation</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +215,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,13 +575,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="18.6640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1">
+      <c r="A29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="4"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="A7:A21"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B29:C31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D7:D21"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D5:D6"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>